<commit_message>
[Feat][other]:Release V1.0 hardware design all need fucntion test pass
</commit_message>
<xml_diff>
--- a/STM32H743VI_Pin_Out/STM32H743VIH_Pin_out.xlsx
+++ b/STM32H743VI_Pin_Out/STM32H743VIH_Pin_out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RI_Morty_WS\Dropbox\pcb_design\NxtPX4\STM32H743VI Pin_Out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622E8522-B84E-4493-A977-354D2C2E7313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981FFDC2-0A64-4761-993A-39A95A42FDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-108" windowWidth="17496" windowHeight="30216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-2910" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN_Define" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="196">
   <si>
     <t>IMU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -788,6 +788,18 @@
   </si>
   <si>
     <t>EXTI15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB Detection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buzzer Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aux GPIO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -876,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,9 +907,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -905,9 +920,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -919,11 +934,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1204,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1218,59 +1232,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="17" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="F4" s="9" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1284,11 +1298,11 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1300,11 +1314,11 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1316,11 +1330,11 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1332,11 +1346,11 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1351,13 +1365,13 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="F9" s="9" t="s">
+      <c r="D9" s="13"/>
+      <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1374,11 +1388,11 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1393,11 +1407,11 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1409,11 +1423,11 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1428,11 +1442,11 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1450,13 +1464,13 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="F14" s="9" t="s">
+      <c r="D14" s="13"/>
+      <c r="F14" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1470,11 +1484,11 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="4" t="s">
         <v>3</v>
       </c>
@@ -1486,11 +1500,11 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1502,11 +1516,11 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="2" t="s">
         <v>189</v>
       </c>
@@ -1518,11 +1532,11 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="2" t="s">
         <v>190</v>
       </c>
@@ -1534,11 +1548,11 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1553,11 +1567,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="2" t="s">
         <v>171</v>
       </c>
@@ -1572,15 +1586,15 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="F21" s="9" t="s">
+      <c r="D21" s="13"/>
+      <c r="F21" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1597,11 +1611,11 @@
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="4" t="s">
         <v>47</v>
       </c>
@@ -1616,11 +1630,11 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="2" t="s">
         <v>50</v>
       </c>
@@ -1638,18 +1652,18 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="14" customHeight="1">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="12"/>
       <c r="E24" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="12" t="s">
         <v>56</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -1666,14 +1680,14 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="14" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="4" t="s">
         <v>59</v>
       </c>
@@ -1688,14 +1702,14 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="4" t="s">
         <v>58</v>
       </c>
@@ -1710,14 +1724,14 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="14" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="E27" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="4" t="s">
         <v>57</v>
       </c>
@@ -1732,14 +1746,14 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="14" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1753,14 +1767,14 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="14" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="4" t="s">
         <v>59</v>
       </c>
@@ -1772,13 +1786,13 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="14" customHeight="1">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="F30" s="9" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="F30" s="12" t="s">
         <v>146</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -1792,11 +1806,11 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="14" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="F31" s="9"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="4" t="s">
         <v>147</v>
       </c>
@@ -1808,15 +1822,15 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="14" customHeight="1">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="F32" s="9" t="s">
+      <c r="D32" s="14"/>
+      <c r="F32" s="12" t="s">
         <v>151</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1830,11 +1844,11 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="14" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="F33" s="12"/>
       <c r="G33" s="4" t="s">
         <v>147</v>
       </c>
@@ -1843,14 +1857,14 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="14" customHeight="1">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="14"/>
       <c r="F34" s="6" t="s">
         <v>159</v>
       </c>
@@ -1863,10 +1877,10 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="14" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
       <c r="F35" s="6" t="s">
         <v>158</v>
       </c>
@@ -1879,10 +1893,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="14" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
       <c r="F36" s="6" t="s">
         <v>157</v>
       </c>
@@ -1902,25 +1916,25 @@
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:11" ht="35">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:11" ht="14" customHeight="1">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="F39" s="9" t="s">
+      <c r="B39" s="9"/>
+      <c r="F39" s="12" t="s">
         <v>30</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -1937,9 +1951,9 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="14" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="F40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="4" t="s">
         <v>3</v>
       </c>
@@ -1954,9 +1968,9 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="14" customHeight="1">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="F41" s="9"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="F41" s="12"/>
       <c r="G41" s="4" t="s">
         <v>6</v>
       </c>
@@ -1971,9 +1985,9 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="14" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="F42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="F42" s="12"/>
       <c r="G42" s="2" t="s">
         <v>34</v>
       </c>
@@ -1988,9 +2002,9 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="14" customHeight="1">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="F43" s="9"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="2" t="s">
         <v>35</v>
       </c>
@@ -2005,9 +2019,9 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="14" customHeight="1">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="F44" s="9"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="F44" s="12"/>
       <c r="G44" s="2" t="s">
         <v>36</v>
       </c>
@@ -2025,9 +2039,9 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="14" customHeight="1">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="F45" s="9"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="F45" s="12"/>
       <c r="G45" s="2" t="s">
         <v>37</v>
       </c>
@@ -2045,8 +2059,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="14" customHeight="1">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
       <c r="F46" s="3" t="s">
         <v>44</v>
       </c>
@@ -2061,11 +2075,11 @@
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="F47" s="9" t="s">
+      <c r="B47" s="9"/>
+      <c r="F47" s="12" t="s">
         <v>71</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -2079,9 +2093,9 @@
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="F48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="4" t="s">
         <v>47</v>
       </c>
@@ -2093,9 +2107,9 @@
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="F49" s="10"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="2" t="s">
         <v>184</v>
       </c>
@@ -2113,11 +2127,11 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="14" customHeight="1">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="F50" s="14" t="s">
+      <c r="B50" s="9"/>
+      <c r="F50" s="17" t="s">
         <v>77</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -2131,9 +2145,9 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="14" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="F51" s="15"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="F51" s="18"/>
       <c r="G51" s="4" t="s">
         <v>79</v>
       </c>
@@ -2145,9 +2159,9 @@
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="F52" s="14" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="F52" s="17" t="s">
         <v>84</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -2161,9 +2175,9 @@
       </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="F53" s="15"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="F53" s="18"/>
       <c r="G53" s="4" t="s">
         <v>79</v>
       </c>
@@ -2175,9 +2189,9 @@
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="F54" s="14" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="F54" s="17" t="s">
         <v>85</v>
       </c>
       <c r="G54" s="4" t="s">
@@ -2191,9 +2205,9 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="F55" s="15"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="F55" s="18"/>
       <c r="G55" s="4" t="s">
         <v>79</v>
       </c>
@@ -2205,9 +2219,9 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="14" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="F56" s="9" t="s">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="F56" s="12" t="s">
         <v>86</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -2224,9 +2238,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="14" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="F57" s="9"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="F57" s="12"/>
       <c r="G57" s="4" t="s">
         <v>79</v>
       </c>
@@ -2241,9 +2255,9 @@
       </c>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="F58" s="9"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="F58" s="12"/>
       <c r="G58" s="4" t="s">
         <v>78</v>
       </c>
@@ -2258,9 +2272,9 @@
       </c>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="F59" s="9" t="s">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="F59" s="12" t="s">
         <v>95</v>
       </c>
       <c r="G59" s="4" t="s">
@@ -2274,9 +2288,9 @@
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="F60" s="9"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="F60" s="12"/>
       <c r="G60" s="4" t="s">
         <v>79</v>
       </c>
@@ -2288,9 +2302,9 @@
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="F61" s="9"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="F61" s="12"/>
       <c r="G61" s="4" t="s">
         <v>78</v>
       </c>
@@ -2302,9 +2316,9 @@
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="F62" s="9" t="s">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="F62" s="12" t="s">
         <v>102</v>
       </c>
       <c r="G62" s="4" t="s">
@@ -2318,9 +2332,9 @@
       </c>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="F63" s="9"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="F63" s="12"/>
       <c r="G63" s="4" t="s">
         <v>79</v>
       </c>
@@ -2332,9 +2346,9 @@
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="F64" s="9"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="F64" s="12"/>
       <c r="G64" s="4" t="s">
         <v>78</v>
       </c>
@@ -2346,11 +2360,11 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="F65" s="12" t="s">
+      <c r="B65" s="9"/>
+      <c r="F65" s="14" t="s">
         <v>104</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -2367,9 +2381,9 @@
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="F66" s="12"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="4" t="s">
         <v>106</v>
       </c>
@@ -2384,11 +2398,11 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="14" customHeight="1">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="8"/>
-      <c r="F67" s="9" t="s">
+      <c r="B67" s="9"/>
+      <c r="F67" s="12" t="s">
         <v>110</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -2402,9 +2416,9 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="14" customHeight="1">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="F68" s="10"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="F68" s="13"/>
       <c r="G68" s="4" t="s">
         <v>113</v>
       </c>
@@ -2416,9 +2430,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="14" customHeight="1">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="F69" s="10"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="F69" s="13"/>
       <c r="G69" s="4" t="s">
         <v>115</v>
       </c>
@@ -2430,9 +2444,9 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="14" customHeight="1">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="F70" s="10"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="F70" s="13"/>
       <c r="G70" s="4" t="s">
         <v>117</v>
       </c>
@@ -2444,9 +2458,9 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="14" customHeight="1">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="F71" s="10"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="F71" s="13"/>
       <c r="G71" s="4" t="s">
         <v>91</v>
       </c>
@@ -2458,9 +2472,9 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="14" customHeight="1">
-      <c r="A72" s="8"/>
-      <c r="B72" s="8"/>
-      <c r="F72" s="10"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="F72" s="13"/>
       <c r="G72" s="4" t="s">
         <v>120</v>
       </c>
@@ -2472,11 +2486,11 @@
       </c>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="F73" s="9" t="s">
+      <c r="B73" s="9"/>
+      <c r="F73" s="12" t="s">
         <v>122</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -2490,9 +2504,9 @@
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
-      <c r="F74" s="10"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="F74" s="13"/>
       <c r="G74" s="4" t="s">
         <v>5</v>
       </c>
@@ -2507,9 +2521,9 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="F75" s="10"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="F75" s="13"/>
       <c r="G75" s="4" t="s">
         <v>124</v>
       </c>
@@ -2521,9 +2535,9 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="F76" s="10"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="F76" s="13"/>
       <c r="G76" s="4" t="s">
         <v>125</v>
       </c>
@@ -2535,9 +2549,9 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="F77" s="10"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="F77" s="13"/>
       <c r="G77" s="4" t="s">
         <v>126</v>
       </c>
@@ -2549,9 +2563,9 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="F78" s="10"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="F78" s="13"/>
       <c r="G78" s="4" t="s">
         <v>127</v>
       </c>
@@ -2563,38 +2577,38 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B79" s="8"/>
-      <c r="F79" s="9" t="s">
+      <c r="B79" s="9"/>
+      <c r="F79" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="H79" s="13" t="s">
+      <c r="H79" s="16" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="F80" s="10"/>
-      <c r="H80" s="13"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="F80" s="13"/>
+      <c r="H80" s="16"/>
       <c r="J80">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="8"/>
-      <c r="B81" s="8"/>
-      <c r="F81" s="10"/>
-      <c r="H81" s="13"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="F81" s="13"/>
+      <c r="H81" s="16"/>
     </row>
     <row r="82" spans="1:11" ht="14" customHeight="1">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="F82" s="10" t="s">
+      <c r="B82" s="9"/>
+      <c r="F82" s="13" t="s">
         <v>138</v>
       </c>
       <c r="G82" s="7" t="s">
@@ -2611,9 +2625,9 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="15" customHeight="1">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="F83" s="10"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="F83" s="13"/>
       <c r="G83" s="4" t="s">
         <v>140</v>
       </c>
@@ -2628,10 +2642,10 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="15" customHeight="1">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="8"/>
+      <c r="B84" s="9"/>
       <c r="F84" t="s">
         <v>164</v>
       </c>
@@ -2646,8 +2660,8 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
       <c r="F85" t="s">
         <v>165</v>
       </c>
@@ -2662,26 +2676,31 @@
       </c>
     </row>
     <row r="88" spans="1:11" ht="14" customHeight="1">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B88" s="8"/>
-      <c r="H88" s="4" t="s">
+      <c r="B88" s="9"/>
+      <c r="F88" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="14" customHeight="1">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="F89" s="19"/>
+      <c r="H89" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="F90" s="19"/>
+      <c r="H90" s="8" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="14" customHeight="1">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="H89" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11">
-      <c r="A90" s="8"/>
-      <c r="B90" s="8"/>
-      <c r="H90" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="J90">
         <v>1</v>
@@ -2691,20 +2710,74 @@
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="H91" s="4" t="s">
-        <v>27</v>
+      <c r="F91" t="s">
+        <v>193</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="H92" s="4" t="s">
+      <c r="F92" t="s">
+        <v>194</v>
+      </c>
+      <c r="H92" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J92">
         <v>1</v>
       </c>
     </row>
+    <row r="94" spans="1:11">
+      <c r="F94" s="19"/>
+      <c r="H94" s="20"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="F95" s="19"/>
+      <c r="H95" s="20"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="F96" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="53">
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="A79:B81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="H79:H81"/>
+    <mergeCell ref="A82:B83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="A50:B64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A67:B72"/>
+    <mergeCell ref="F67:F72"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="A73:B78"/>
+    <mergeCell ref="F73:F78"/>
+    <mergeCell ref="A24:B29"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="A47:B49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="A4:B20"/>
+    <mergeCell ref="A21:B23"/>
+    <mergeCell ref="A39:B46"/>
+    <mergeCell ref="A34:B36"/>
+    <mergeCell ref="C34:D36"/>
     <mergeCell ref="A88:B90"/>
     <mergeCell ref="A84:B85"/>
     <mergeCell ref="F2:J2"/>
@@ -2721,41 +2794,6 @@
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="C4:D8"/>
     <mergeCell ref="C9:D13"/>
-    <mergeCell ref="A24:B29"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="A47:B49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="A4:B20"/>
-    <mergeCell ref="A21:B23"/>
-    <mergeCell ref="A39:B46"/>
-    <mergeCell ref="A34:B36"/>
-    <mergeCell ref="C34:D36"/>
-    <mergeCell ref="H79:H81"/>
-    <mergeCell ref="A82:B83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="F62:F64"/>
-    <mergeCell ref="A50:B64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A67:B72"/>
-    <mergeCell ref="F67:F72"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="A73:B78"/>
-    <mergeCell ref="F73:F78"/>
-    <mergeCell ref="A79:B81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="F32:F33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>